<commit_message>
Phúc mằn thử thôi nha
</commit_message>
<xml_diff>
--- a/gia_nguyen_lieu.xlsx
+++ b/gia_nguyen_lieu.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aaeeecda4e97f96c/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\quantrong\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="98" documentId="8_{83691E01-40D5-4923-9E79-A19EB1AF3D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{941528A8-9300-42B8-8564-AD3FD4A75B39}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F593E0-1573-4354-B1AB-1C8785053468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="3375" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{39965E9C-9B91-4D2A-A674-BC6DBB3A2ECE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39965E9C-9B91-4D2A-A674-BC6DBB3A2ECE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Giá Bột Sắt" sheetId="1" r:id="rId1"/>
-    <sheet name="Giá Than Cốt" sheetId="2" r:id="rId2"/>
-    <sheet name="Giá Cốt Thép" sheetId="3" r:id="rId3"/>
+    <sheet name="gia_bot_sat" sheetId="1" r:id="rId1"/>
+    <sheet name="gia_than_coc" sheetId="2" r:id="rId2"/>
+    <sheet name="gia_cot_thep" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -78,7 +78,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,18 +117,18 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
-    <cellStyle name="Dấu phẩy" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -7250,8 +7250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC8431B-B7A5-4975-9F97-C1B0E8F33B54}">
   <dimension ref="A1:I120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>